<commit_message>
juda xursanman xuyyet qivorgudek
</commit_message>
<xml_diff>
--- a/public/Super_кв-2_2024_nalog.xlsx
+++ b/public/Super_кв-2_2024_nalog.xlsx
@@ -418,21 +418,21 @@
         <v>Налог на доходы (прибыль) с юрид.лиц.</v>
       </c>
       <c r="B2">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
         <v>Налог на доходы  физических лиц.</v>
       </c>
-      <c r="B3" t="str">
-        <v/>
-      </c>
-      <c r="C3" t="str">
-        <v/>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
       </c>
     </row>
     <row r="4">

</xml_diff>